<commit_message>
include Prezi link in Word doc
</commit_message>
<xml_diff>
--- a/MLModelAvg4Tableau.xlsx
+++ b/MLModelAvg4Tableau.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dianeshomefolder/Documents/git/meteorite-classification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{47E6F050-361D-9E48-9400-30A4E36CFE61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F487369B-6CC3-E54D-8AC8-3F8369538F9A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="15960" xr2:uid="{15A8D31F-F60A-3C47-A0E2-257001C8FFE5}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="27640" windowHeight="15960" xr2:uid="{15A8D31F-F60A-3C47-A0E2-257001C8FFE5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -468,7 +468,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>93.7</v>
+        <v>93.8</v>
       </c>
     </row>
     <row r="8" spans="1:2">

</xml_diff>